<commit_message>
finished week 7, started week 8
</commit_message>
<xml_diff>
--- a/Grades_MSDS660.xlsx
+++ b/Grades_MSDS660.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9676edfc3f3b3502/Documents/School/_REGIS/2022-05_Summer/MSDS660/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{6588BF20-2B25-4BF5-9AED-5219590276EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC874882-F4EE-415B-A46D-4FF705C3C182}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{6588BF20-2B25-4BF5-9AED-5219590276EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C57D162-018D-4AB8-B15E-B879775E027C}"/>
   <bookViews>
     <workbookView xWindow="1833" yWindow="1833" windowWidth="19200" windowHeight="10074" xr2:uid="{73165B4B-521D-47CD-9CC0-B7015BE7127C}"/>
   </bookViews>
@@ -404,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937082C1-A858-45CD-A3A7-68FFB721921E}">
-  <dimension ref="B5:K26"/>
+  <dimension ref="B5:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -497,14 +497,23 @@
       <c r="E8">
         <v>10</v>
       </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
       <c r="G8">
         <v>10</v>
       </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="J8">
         <v>10</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.5">
@@ -515,11 +524,26 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <v>15</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
       <c r="H9">
         <v>15</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
       </c>
       <c r="K9">
         <v>15</v>
@@ -531,230 +555,256 @@
         <v>100</v>
       </c>
     </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B13" t="s">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
         <v>4</v>
       </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <f>SUM(D14:K14)</f>
+        <v>6.75</v>
+      </c>
       <c r="D14">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>0.75</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>0.75</v>
       </c>
       <c r="G14">
-        <v>4</v>
+        <f t="shared" ref="G14" si="2">F14</f>
+        <v>0.75</v>
       </c>
       <c r="H14">
-        <v>5</v>
+        <f t="shared" ref="H14" si="3">G14</f>
+        <v>0.75</v>
       </c>
       <c r="I14">
-        <v>6</v>
+        <f t="shared" ref="I14" si="4">H14</f>
+        <v>0.75</v>
       </c>
       <c r="J14">
-        <v>7</v>
+        <f t="shared" ref="J14" si="5">I14</f>
+        <v>0.75</v>
       </c>
       <c r="K14">
-        <v>8</v>
+        <f t="shared" ref="K14" si="6">J14</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <f>SUM(D15:K15)</f>
-        <v>9.75</v>
+        <f t="shared" ref="C15:C16" si="7">SUM(D15:K15)</f>
+        <v>37.5</v>
       </c>
       <c r="D15">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>0.75</v>
+        <v>10</v>
       </c>
       <c r="F15">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.75</v>
+        <v>9.5</v>
       </c>
       <c r="H15">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" ref="H15:K15" si="2">H15</f>
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="J15">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>5</v>
       </c>
       <c r="K15">
-        <f t="shared" si="2"/>
-        <v>1.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="7"/>
+        <v>36.450000000000003</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>14.25</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>14.7</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="C17">
+        <f>SUM(C14:C16)</f>
+        <v>80.7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="D23">
         <v>1</v>
       </c>
-      <c r="C16">
-        <f t="shared" ref="C16:C17" si="3">SUM(D16:K16)</f>
-        <v>41.5</v>
-      </c>
-      <c r="D16">
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="G16">
-        <v>9.5</v>
-      </c>
-      <c r="I16">
-        <v>9.5</v>
-      </c>
-      <c r="J16">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="3"/>
-        <v>42.5</v>
-      </c>
-      <c r="F17">
-        <v>14.25</v>
-      </c>
-      <c r="H17">
-        <v>14.25</v>
-      </c>
-      <c r="K17">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="C18">
-        <f>SUM(C15:C17)</f>
-        <v>93.75</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B21" t="s">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>3</v>
-      </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22">
-        <v>5</v>
-      </c>
-      <c r="I22">
+      <c r="I23">
         <v>6</v>
       </c>
-      <c r="J22">
+      <c r="J23">
         <v>7</v>
       </c>
-      <c r="K22">
+      <c r="K23">
         <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="B23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <f>SUM(D23:K23)</f>
-        <v>9</v>
-      </c>
-      <c r="D23">
-        <v>1.5</v>
-      </c>
-      <c r="E23">
-        <v>0.75</v>
-      </c>
-      <c r="F23">
-        <v>0.75</v>
-      </c>
-      <c r="G23">
-        <v>0.75</v>
-      </c>
-      <c r="H23">
-        <v>0.75</v>
-      </c>
-      <c r="I23">
-        <v>1.5</v>
-      </c>
-      <c r="J23">
-        <v>1.5</v>
-      </c>
-      <c r="K23">
-        <v>1.5</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
-        <f t="shared" ref="C24:C25" si="4">SUM(D24:K24)</f>
-        <v>40.5</v>
+        <f>SUM(D24:K24)</f>
+        <v>9</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>0.75</v>
+      </c>
+      <c r="F24">
+        <v>0.75</v>
       </c>
       <c r="G24">
-        <v>9.5</v>
+        <v>0.75</v>
+      </c>
+      <c r="H24">
+        <v>0.75</v>
       </c>
       <c r="I24">
-        <v>9</v>
+        <v>1.5</v>
       </c>
       <c r="J24">
-        <v>9</v>
+        <v>1.5</v>
+      </c>
+      <c r="K24">
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C26" si="8">SUM(D25:K25)</f>
+        <v>40.5</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>9.5</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="B26" t="s">
         <v>2</v>
       </c>
-      <c r="C25">
-        <f t="shared" si="4"/>
+      <c r="C26">
+        <f t="shared" si="8"/>
         <v>34.25</v>
       </c>
-      <c r="F25">
+      <c r="F26">
         <v>14.25</v>
       </c>
-      <c r="H25">
+      <c r="H26">
         <v>10</v>
       </c>
-      <c r="K25">
+      <c r="K26">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.5">
-      <c r="C26">
-        <f>SUM(C23:C25)</f>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.5">
+      <c r="C27">
+        <f>SUM(C24:C26)</f>
         <v>83.75</v>
       </c>
     </row>

</xml_diff>